<commit_message>
Completed code, documentation & runtime tests for serial implementation
</commit_message>
<xml_diff>
--- a/gioia/code/runtime.xlsx
+++ b/gioia/code/runtime.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="13540" yWindow="0" windowWidth="37660" windowHeight="27180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="35">
   <si>
     <t>Pre-processing</t>
   </si>
@@ -84,28 +84,46 @@
     <t>4 potential errors</t>
   </si>
   <si>
-    <t>320KB+8.6MB
-+4.5MB+731KB</t>
-  </si>
-  <si>
-    <t>941B</t>
-  </si>
-  <si>
-    <t>Shuffle reads</t>
-  </si>
-  <si>
-    <t>Shuffle writes</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>10 shuffles
-(2.5KB-15.1KB)</t>
-  </si>
-  <si>
-    <t>11 shuffles
-(2.5KB-8.9KB)</t>
+    <t>tiny.txt</t>
+  </si>
+  <si>
+    <t>OCRsample.txt</t>
+  </si>
+  <si>
+    <t>yelp10reviews.txt</t>
+  </si>
+  <si>
+    <t>yelp100reviews.txt</t>
+  </si>
+  <si>
+    <t>1,467 words</t>
+  </si>
+  <si>
+    <t>209 words</t>
+  </si>
+  <si>
+    <t>700 words</t>
+  </si>
+  <si>
+    <t>4 errors identified</t>
+  </si>
+  <si>
+    <t>0 errors identified</t>
+  </si>
+  <si>
+    <t>175 errors identified</t>
+  </si>
+  <si>
+    <t>241 errors identified</t>
+  </si>
+  <si>
+    <t>12,029 words</t>
+  </si>
+  <si>
+    <t>1,761 errors identified</t>
+  </si>
+  <si>
+    <t>NOTES ON OPTIMIZATIONS</t>
   </si>
 </sst>
 </file>
@@ -155,7 +173,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -170,18 +188,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -189,8 +201,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="93">
+  <cellStyleXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -284,8 +305,66 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -314,23 +393,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="93">
+  <cellStyles count="151">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -377,6 +450,35 @@
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -423,6 +525,35 @@
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -752,18 +883,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H43"/>
+  <dimension ref="B2:L70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
     <col min="2" max="2" width="40.83203125" customWidth="1"/>
-    <col min="3" max="4" width="18.83203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="40.83203125" customWidth="1"/>
-    <col min="7" max="8" width="18.83203125" style="3" customWidth="1"/>
+    <col min="3" max="8" width="18.83203125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" customWidth="1"/>
+    <col min="10" max="10" width="18.83203125" style="3" hidden="1"/>
+    <col min="12" max="12" width="18.83203125" hidden="1"/>
+    <col min="13" max="16384" width="10.83203125" hidden="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8">
@@ -772,9 +904,8 @@
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
-      <c r="F2" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
     </row>
@@ -785,18 +916,13 @@
       <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>2</v>
-      </c>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
     </row>
     <row r="5" spans="2:8" s="1" customFormat="1">
       <c r="C5" s="5" t="s">
@@ -805,11 +931,17 @@
       <c r="D5" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="E5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="G5" s="5" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:8" s="1" customFormat="1">
@@ -819,47 +951,74 @@
       <c r="D6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
+      <c r="E6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="7" spans="2:8" s="1" customFormat="1">
       <c r="C7" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="8" spans="2:8" s="1" customFormat="1">
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="2:8" s="13" customFormat="1">
+    <row r="9" spans="2:8" s="12" customFormat="1">
       <c r="B9" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="13">
         <f>AVERAGE(C10:C14)</f>
-        <v>34.198</v>
-      </c>
-      <c r="D9" s="16">
+        <v>34.54</v>
+      </c>
+      <c r="D9" s="13">
         <f>AVERAGE(D10:D14)</f>
-        <v>0.84000000000000008</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9" s="16" t="e">
-        <f>AVERAGE(G10:G14)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H9" s="16" t="e">
-        <f>AVERAGE(H10:H14)</f>
-        <v>#DIV/0!</v>
+        <v>0.84600000000000009</v>
+      </c>
+      <c r="E9" s="13">
+        <f>AVERAGE(E10:E14)</f>
+        <v>5.2739999999999991</v>
+      </c>
+      <c r="F9" s="13">
+        <f>AVERAGE(F10:F14)</f>
+        <v>15.75</v>
+      </c>
+      <c r="G9" s="13">
+        <f t="shared" ref="G9:H9" si="0">AVERAGE(G10:G14)</f>
+        <v>36.897999999999996</v>
+      </c>
+      <c r="H9" s="13">
+        <f t="shared" si="0"/>
+        <v>323.74200000000002</v>
       </c>
     </row>
     <row r="10" spans="2:8">
@@ -867,524 +1026,764 @@
         <v>8</v>
       </c>
       <c r="C10" s="7">
-        <v>34.39</v>
+        <v>33.090000000000003</v>
       </c>
       <c r="D10" s="7">
-        <v>0.8</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+        <v>0.79</v>
+      </c>
+      <c r="E10" s="7">
+        <v>5.61</v>
+      </c>
+      <c r="F10" s="7">
+        <v>15.7</v>
+      </c>
+      <c r="G10" s="7">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="H10" s="7">
+        <v>314.55</v>
+      </c>
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="7">
-        <v>34.24</v>
+        <v>37.380000000000003</v>
       </c>
       <c r="D11" s="7">
         <v>0.89</v>
       </c>
-      <c r="F11" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
+      <c r="E11" s="7">
+        <v>5.44</v>
+      </c>
+      <c r="F11" s="7">
+        <v>15.52</v>
+      </c>
+      <c r="G11" s="7">
+        <v>36.43</v>
+      </c>
+      <c r="H11" s="7">
+        <v>326.73</v>
+      </c>
     </row>
     <row r="12" spans="2:8">
       <c r="B12" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="7">
-        <v>34.06</v>
+        <v>34.01</v>
       </c>
       <c r="D12" s="7">
-        <v>0.83</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
+        <v>0.85</v>
+      </c>
+      <c r="E12" s="7">
+        <v>5.17</v>
+      </c>
+      <c r="F12" s="7">
+        <v>15.78</v>
+      </c>
+      <c r="G12" s="7">
+        <v>37.86</v>
+      </c>
+      <c r="H12" s="7">
+        <v>321.48</v>
+      </c>
     </row>
     <row r="13" spans="2:8">
       <c r="B13" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="7">
-        <v>33.85</v>
+        <v>34.25</v>
       </c>
       <c r="D13" s="7">
-        <v>0.79</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
+        <v>0.85</v>
+      </c>
+      <c r="E13" s="7">
+        <v>5.08</v>
+      </c>
+      <c r="F13" s="7">
+        <v>16.559999999999999</v>
+      </c>
+      <c r="G13" s="7">
+        <v>36.43</v>
+      </c>
+      <c r="H13" s="7">
+        <v>325.32</v>
+      </c>
     </row>
     <row r="14" spans="2:8">
       <c r="B14" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="7">
-        <v>34.450000000000003</v>
+        <v>33.97</v>
       </c>
       <c r="D14" s="7">
-        <v>0.89</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
+        <v>0.85</v>
+      </c>
+      <c r="E14" s="7">
+        <v>5.07</v>
+      </c>
+      <c r="F14" s="7">
+        <v>15.19</v>
+      </c>
+      <c r="G14" s="7">
+        <v>37.47</v>
+      </c>
+      <c r="H14" s="7">
+        <v>330.63</v>
+      </c>
     </row>
     <row r="15" spans="2:8">
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="2:8" s="13" customFormat="1">
+    <row r="16" spans="2:8" s="12" customFormat="1">
       <c r="B16" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="16">
-        <f>AVERAGE(C19:C23)</f>
-        <v>53.486000000000004</v>
-      </c>
-      <c r="D16" s="16">
-        <f>AVERAGE(D19:D23)</f>
-        <v>22.148</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="G16" s="16" t="e">
-        <f>AVERAGE(G19:G23)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H16" s="16" t="e">
-        <f>AVERAGE(H19:H23)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" s="13" customFormat="1" ht="30">
-      <c r="B17" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" s="12"/>
-      <c r="H17" s="15"/>
-    </row>
-    <row r="18" spans="2:8" s="13" customFormat="1" ht="30">
-      <c r="B18" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G18" s="12"/>
-      <c r="H18" s="15"/>
+      <c r="C16" s="13" t="e">
+        <f>AVERAGE(C17:C21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D16" s="13" t="e">
+        <f>AVERAGE(D17:D21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E16" s="13" t="e">
+        <f>AVERAGE(E17:E21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F16" s="13" t="e">
+        <f>AVERAGE(F17:F21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G16" s="13" t="e">
+        <f>AVERAGE(G17:G21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H16" s="13" t="e">
+        <f>AVERAGE(H17:H21)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="B17" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="2:8">
+      <c r="B18" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
     </row>
     <row r="19" spans="2:8">
       <c r="B19" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="7">
-        <v>52.77</v>
-      </c>
-      <c r="D19" s="7">
-        <v>21.7</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>8</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
     </row>
     <row r="20" spans="2:8">
       <c r="B20" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="7">
-        <v>52.76</v>
-      </c>
-      <c r="D20" s="7">
-        <v>23.27</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>9</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
     </row>
     <row r="21" spans="2:8">
       <c r="B21" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="7">
-        <v>54.32</v>
-      </c>
-      <c r="D21" s="7">
-        <v>21.54</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>10</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
     </row>
     <row r="22" spans="2:8">
-      <c r="B22" s="8" t="s">
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="2:8" s="12" customFormat="1">
+      <c r="B23" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="13" t="e">
+        <f>AVERAGE(C24:C28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D23" s="13" t="e">
+        <f>AVERAGE(D24:D28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E23" s="13" t="e">
+        <f>AVERAGE(E24:E28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F23" s="13" t="e">
+        <f>AVERAGE(F24:F28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G23" s="13" t="e">
+        <f>AVERAGE(G24:G28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H23" s="13" t="e">
+        <f>AVERAGE(H24:H28)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8">
+      <c r="B24" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="B25" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="B26" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+    </row>
+    <row r="27" spans="2:8">
+      <c r="B27" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="7">
-        <v>53.9</v>
-      </c>
-      <c r="D22" s="7">
-        <v>22.87</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-    </row>
-    <row r="23" spans="2:8">
-      <c r="B23" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" s="7">
-        <v>53.68</v>
-      </c>
-      <c r="D23" s="7">
-        <v>21.36</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-    </row>
-    <row r="24" spans="2:8">
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-    </row>
-    <row r="25" spans="2:8" s="13" customFormat="1">
-      <c r="B25" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="16">
-        <f>AVERAGE(C28:C32)</f>
-        <v>53.55</v>
-      </c>
-      <c r="D25" s="16">
-        <f>AVERAGE(D28:D32)</f>
-        <v>27.9</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G25" s="16" t="e">
-        <f>AVERAGE(G28:G32)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H25" s="16" t="e">
-        <f>AVERAGE(H28:H32)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" s="13" customFormat="1" ht="30">
-      <c r="B26" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G26" s="12"/>
-      <c r="H26" s="15"/>
-    </row>
-    <row r="27" spans="2:8" s="13" customFormat="1" ht="30">
-      <c r="B27" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F27" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G27" s="12"/>
-      <c r="H27" s="15"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
     </row>
     <row r="28" spans="2:8">
       <c r="B28" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C28" s="7">
-        <v>53.27</v>
-      </c>
-      <c r="D28" s="7">
-        <v>27.8</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>8</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
     </row>
     <row r="29" spans="2:8">
-      <c r="B29" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="7">
-        <v>53.48</v>
-      </c>
-      <c r="D29" s="7">
-        <v>28.15</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-    </row>
-    <row r="30" spans="2:8">
-      <c r="B30" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" s="7">
-        <v>50.44</v>
-      </c>
-      <c r="D30" s="7">
-        <v>27.56</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="2:8" s="12" customFormat="1">
+      <c r="B30" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="13" t="e">
+        <f>AVERAGE(C31:C35)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D30" s="13" t="e">
+        <f>AVERAGE(D31:D35)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E30" s="13" t="e">
+        <f>AVERAGE(E31:E35)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F30" s="13" t="e">
+        <f>AVERAGE(F31:F35)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G30" s="13" t="e">
+        <f>AVERAGE(G31:G35)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H30" s="13" t="e">
+        <f>AVERAGE(H31:H35)</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="31" spans="2:8">
       <c r="B31" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C31" s="7">
-        <v>55.04</v>
-      </c>
-      <c r="D31" s="7">
-        <v>27.95</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>11</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
     </row>
     <row r="32" spans="2:8">
       <c r="B32" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C32" s="7">
-        <v>55.52</v>
-      </c>
-      <c r="D32" s="7">
-        <v>28.04</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>12</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
     </row>
     <row r="33" spans="2:8">
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-    </row>
-    <row r="34" spans="2:8" s="13" customFormat="1">
-      <c r="B34" s="11" t="s">
+      <c r="B33" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+    </row>
+    <row r="34" spans="2:8">
+      <c r="B34" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+    </row>
+    <row r="35" spans="2:8">
+      <c r="B35" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+    </row>
+    <row r="36" spans="2:8">
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+    </row>
+    <row r="37" spans="2:8">
+      <c r="B37" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+    </row>
+    <row r="40" spans="2:8">
+      <c r="B40" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+    </row>
+    <row r="42" spans="2:8">
+      <c r="B42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+    </row>
+    <row r="43" spans="2:8">
+      <c r="B43" s="1"/>
+      <c r="C43" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8">
+      <c r="B44" s="1"/>
+      <c r="C44" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H44" s="5"/>
+    </row>
+    <row r="45" spans="2:8">
+      <c r="B45" s="1"/>
+      <c r="C45" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+    </row>
+    <row r="46" spans="2:8">
+      <c r="B46" s="1"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+    </row>
+    <row r="47" spans="2:8">
+      <c r="B47" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" s="13" t="e">
+        <f>AVERAGE(C48:C52)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D47" s="13" t="e">
+        <f>AVERAGE(D48:D52)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E47" s="13" t="e">
+        <f>AVERAGE(E48:E52)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F47" s="13" t="e">
+        <f>AVERAGE(F48:F52)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G47" s="13" t="e">
+        <f>AVERAGE(G48:G52)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H47" s="13" t="e">
+        <f>AVERAGE(H48:H52)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8">
+      <c r="B48" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
+    </row>
+    <row r="49" spans="2:8">
+      <c r="B49" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
+    </row>
+    <row r="50" spans="2:8">
+      <c r="B50" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
+    </row>
+    <row r="51" spans="2:8">
+      <c r="B51" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="7"/>
+    </row>
+    <row r="52" spans="2:8">
+      <c r="B52" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="7"/>
+    </row>
+    <row r="53" spans="2:8">
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+    </row>
+    <row r="54" spans="2:8">
+      <c r="B54" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C54" s="13" t="e">
+        <f>AVERAGE(C55:C59)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D54" s="13" t="e">
+        <f>AVERAGE(D55:D59)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E54" s="13" t="e">
+        <f>AVERAGE(E55:E59)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F54" s="13" t="e">
+        <f>AVERAGE(F55:F59)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G54" s="13" t="e">
+        <f>AVERAGE(G55:G59)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H54" s="13" t="e">
+        <f>AVERAGE(H55:H59)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8">
+      <c r="B55" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="7"/>
+    </row>
+    <row r="56" spans="2:8">
+      <c r="B56" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C56" s="7"/>
+      <c r="D56" s="7"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="7"/>
+    </row>
+    <row r="57" spans="2:8">
+      <c r="B57" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C57" s="7"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="7"/>
+    </row>
+    <row r="58" spans="2:8">
+      <c r="B58" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C58" s="7"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
+      <c r="H58" s="7"/>
+    </row>
+    <row r="59" spans="2:8">
+      <c r="B59" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C59" s="7"/>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="7"/>
+      <c r="H59" s="7"/>
+    </row>
+    <row r="60" spans="2:8">
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+    </row>
+    <row r="61" spans="2:8">
+      <c r="B61" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="16">
-        <f>AVERAGE(C37:C41)</f>
-        <v>52.132000000000005</v>
-      </c>
-      <c r="D34" s="16">
-        <f>AVERAGE(D37:D41)</f>
-        <v>37.766000000000005</v>
-      </c>
-      <c r="F34" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="G34" s="16" t="e">
-        <f>AVERAGE(G37:G41)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H34" s="16" t="e">
-        <f>AVERAGE(H37:H41)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" s="13" customFormat="1" ht="30">
-      <c r="B35" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F35" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G35" s="12"/>
-      <c r="H35" s="15"/>
-    </row>
-    <row r="36" spans="2:8" s="13" customFormat="1" ht="30">
-      <c r="B36" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F36" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G36" s="12"/>
-      <c r="H36" s="15"/>
-    </row>
-    <row r="37" spans="2:8">
-      <c r="B37" s="8" t="s">
+      <c r="C61" s="13" t="e">
+        <f>AVERAGE(C62:C66)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D61" s="13" t="e">
+        <f>AVERAGE(D62:D66)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E61" s="13" t="e">
+        <f>AVERAGE(E62:E66)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F61" s="13" t="e">
+        <f>AVERAGE(F62:F66)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G61" s="13" t="e">
+        <f>AVERAGE(G62:G66)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H61" s="13" t="e">
+        <f>AVERAGE(H62:H66)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8">
+      <c r="B62" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C37" s="7">
-        <v>52.48</v>
-      </c>
-      <c r="D37" s="7">
-        <v>38</v>
-      </c>
-      <c r="F37" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
-    </row>
-    <row r="38" spans="2:8">
-      <c r="B38" s="8" t="s">
+      <c r="C62" s="7"/>
+      <c r="D62" s="7"/>
+    </row>
+    <row r="63" spans="2:8">
+      <c r="B63" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C38" s="7">
-        <v>52</v>
-      </c>
-      <c r="D38" s="7">
-        <v>37.93</v>
-      </c>
-      <c r="F38" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-    </row>
-    <row r="39" spans="2:8">
-      <c r="B39" s="8" t="s">
+      <c r="C63" s="7"/>
+      <c r="D63" s="7"/>
+    </row>
+    <row r="64" spans="2:8">
+      <c r="B64" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C39" s="7">
-        <v>52.24</v>
-      </c>
-      <c r="D39" s="7">
-        <v>38.130000000000003</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-    </row>
-    <row r="40" spans="2:8">
-      <c r="B40" s="8" t="s">
+      <c r="C64" s="7"/>
+      <c r="D64" s="7"/>
+    </row>
+    <row r="65" spans="2:8">
+      <c r="B65" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C40" s="7">
-        <v>53.56</v>
-      </c>
-      <c r="D40" s="7">
-        <v>37.24</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
-    </row>
-    <row r="41" spans="2:8">
-      <c r="B41" s="8" t="s">
+      <c r="C65" s="7"/>
+      <c r="D65" s="7"/>
+    </row>
+    <row r="66" spans="2:8">
+      <c r="B66" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C41" s="7">
-        <v>50.38</v>
-      </c>
-      <c r="D41" s="7">
-        <v>37.53</v>
-      </c>
-      <c r="F41" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7"/>
-    </row>
-    <row r="42" spans="2:8">
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
-    </row>
-    <row r="43" spans="2:8">
-      <c r="B43" s="6" t="s">
+      <c r="C66" s="7"/>
+      <c r="D66" s="7"/>
+    </row>
+    <row r="67" spans="2:8">
+      <c r="C67" s="4"/>
+      <c r="D67" s="4"/>
+    </row>
+    <row r="68" spans="2:8">
+      <c r="B68" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="F43" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
+      <c r="C68" s="4"/>
+      <c r="D68" s="4"/>
+    </row>
+    <row r="70" spans="2:8">
+      <c r="B70" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C70" s="10"/>
+      <c r="D70" s="10"/>
+      <c r="E70" s="10"/>
+      <c r="F70" s="10"/>
+      <c r="G70" s="10"/>
+      <c r="H70" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
SPARK v3 working again :)
</commit_message>
<xml_diff>
--- a/gioia/code/runtime.xlsx
+++ b/gioia/code/runtime.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -191,7 +191,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -222,6 +222,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -526,7 +532,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -605,6 +611,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1223,8 +1232,8 @@
   <dimension ref="A2:R97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="18" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J6" sqref="J6"/>
+      <pane ySplit="18" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H85" sqref="H85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2573,17 +2582,17 @@
         <f>E$6/E82</f>
         <v>13.730874852883485</v>
       </c>
-      <c r="F81" s="29" t="e">
+      <c r="F81" s="29">
         <f t="shared" ref="F81" si="20">F$6/F82</f>
-        <v>#DIV/0!</v>
+        <v>2.2005772005772006</v>
       </c>
       <c r="G81" s="29">
         <f t="shared" ref="G81" si="21">G$6/G82</f>
-        <v>23.226725775807473</v>
+        <v>16.113206165562186</v>
       </c>
       <c r="H81" s="29">
         <f t="shared" ref="H81" si="22">H$6/H82</f>
-        <v>59.442097200602866</v>
+        <v>45.70925534205626</v>
       </c>
       <c r="I81" s="29" t="e">
         <f t="shared" ref="I81" si="23">I$6/I82</f>
@@ -2606,17 +2615,17 @@
         <f t="shared" si="25"/>
         <v>50.98</v>
       </c>
-      <c r="F82" s="13" t="e">
+      <c r="F82" s="13">
         <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
+        <v>83.16</v>
       </c>
       <c r="G82" s="13">
         <f t="shared" si="25"/>
-        <v>63.16</v>
+        <v>91.043333333333337</v>
       </c>
       <c r="H82" s="13">
         <f t="shared" si="25"/>
-        <v>202.36500000000001</v>
+        <v>263.16333333333336</v>
       </c>
       <c r="I82" s="13" t="e">
         <f>AVERAGE(I83:I87)</f>
@@ -2637,7 +2646,9 @@
       <c r="E83" s="7">
         <v>50.98</v>
       </c>
-      <c r="F83" s="7"/>
+      <c r="F83" s="30">
+        <v>83.16</v>
+      </c>
       <c r="G83" s="7">
         <v>63.33</v>
       </c>
@@ -2674,8 +2685,12 @@
       </c>
       <c r="E85" s="7"/>
       <c r="F85" s="7"/>
-      <c r="G85" s="7"/>
-      <c r="H85" s="7"/>
+      <c r="G85" s="30">
+        <v>146.81</v>
+      </c>
+      <c r="H85" s="30">
+        <v>384.76</v>
+      </c>
       <c r="I85" s="7"/>
       <c r="J85" s="7"/>
     </row>

</xml_diff>

<commit_message>
Prelim work on notebook submission
</commit_message>
<xml_diff>
--- a/gioia/code/runtime.xlsx
+++ b/gioia/code/runtime.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="45">
   <si>
     <t>Pre-processing</t>
   </si>
@@ -111,9 +111,6 @@
     <t>Not enough memory.</t>
   </si>
   <si>
-    <t>8 executors, 4 cores, 16 partitions</t>
-  </si>
-  <si>
     <t>8 executors, 4 cores, 64 partitions</t>
   </si>
   <si>
@@ -147,10 +144,16 @@
     <t>6.5MB</t>
   </si>
   <si>
-    <t>64 executors, 4 cores, 256 partitions</t>
-  </si>
-  <si>
-    <t>Didn't finish running</t>
+    <t>`</t>
+  </si>
+  <si>
+    <t>16 executors, 4 cores, 256 partitions</t>
+  </si>
+  <si>
+    <t>File is too big.</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -222,7 +225,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -243,7 +246,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="-0.499984740745262"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -277,7 +286,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="643">
+  <cellStyleXfs count="701">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -921,8 +930,66 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -970,7 +1037,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -993,7 +1059,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1002,9 +1067,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1017,14 +1079,34 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="3" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="643">
+  <cellStyles count="701">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1346,6 +1428,35 @@
     <cellStyle name="Followed Hyperlink" xfId="638" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="640" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="642" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="644" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="646" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="648" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="650" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="652" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="654" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="656" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="658" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="660" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="662" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="664" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="666" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="668" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="670" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="672" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="674" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="676" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="678" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="680" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="682" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="684" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="686" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="688" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="690" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="692" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="694" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="696" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="698" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="700" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1667,6 +1778,35 @@
     <cellStyle name="Hyperlink" xfId="637" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="639" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="641" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="643" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="645" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="647" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="649" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="651" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="653" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="655" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="657" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="659" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="661" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="663" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="665" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="667" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="669" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="671" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="673" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="675" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="677" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="679" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="681" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="683" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="685" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="687" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="689" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="691" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="693" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="695" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="697" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="699" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1996,11 +2136,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:V75"/>
+  <dimension ref="A2:X83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <pane ySplit="8" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G79" sqref="G79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2017,7 +2157,8 @@
     <col min="16" max="16" width="18.83203125" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="0" hidden="1" customWidth="1"/>
     <col min="18" max="22" width="18.83203125" hidden="1" customWidth="1"/>
-    <col min="23" max="16384" width="10.83203125" hidden="1"/>
+    <col min="23" max="24" width="18.83203125" hidden="1"/>
+    <col min="25" max="16384" width="10.83203125" hidden="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:14">
@@ -2073,7 +2214,7 @@
         <v>26</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="2:14" s="1" customFormat="1">
@@ -2135,29 +2276,29 @@
     <row r="8" spans="2:14" s="1" customFormat="1">
       <c r="C8" s="5"/>
       <c r="D8" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="H8" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="I8" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="J8" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="J8" s="15" t="s">
+      <c r="K8" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="K8" s="15" t="s">
+      <c r="L8" s="15" t="s">
         <v>39</v>
-      </c>
-      <c r="L8" s="15" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="9" spans="2:14" s="1" customFormat="1">
@@ -2212,110 +2353,112 @@
       <c r="B13" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="35">
+      <c r="C13" s="33"/>
+      <c r="D13" s="32">
         <v>32.47</v>
       </c>
-      <c r="E13" s="36"/>
-      <c r="F13" s="35">
+      <c r="E13" s="33"/>
+      <c r="F13" s="32">
         <v>4.8600000000000003</v>
       </c>
-      <c r="G13" s="35">
+      <c r="G13" s="32">
         <v>35.85</v>
       </c>
-      <c r="H13" s="35">
+      <c r="H13" s="32">
         <v>313.16000000000003</v>
       </c>
-      <c r="I13" s="35">
+      <c r="I13" s="32">
         <v>813.04</v>
       </c>
-      <c r="J13" s="35">
+      <c r="J13" s="32">
         <v>1639.38</v>
       </c>
-      <c r="K13" s="35"/>
-      <c r="L13" s="35"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
     </row>
     <row r="14" spans="2:14" s="1" customFormat="1">
       <c r="B14" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="35">
+      <c r="C14" s="29"/>
+      <c r="D14" s="32">
         <v>33.79</v>
       </c>
-      <c r="E14" s="31"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35">
+      <c r="E14" s="29"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32">
         <v>1611.21</v>
       </c>
-      <c r="K14" s="35"/>
-      <c r="L14" s="35"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
     </row>
     <row r="15" spans="2:14" ht="16" thickBot="1">
-      <c r="B15" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="29">
+      <c r="B15" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="33"/>
+      <c r="D15" s="27">
         <f>MIN(D13:D14)</f>
         <v>32.47</v>
       </c>
-      <c r="E15" s="28"/>
-      <c r="F15" s="29">
+      <c r="E15" s="33"/>
+      <c r="F15" s="27">
         <f t="shared" ref="F15" si="0">MIN(F13:F14)</f>
         <v>4.8600000000000003</v>
       </c>
-      <c r="G15" s="29">
+      <c r="G15" s="27">
         <f t="shared" ref="G15" si="1">MIN(G13:G14)</f>
         <v>35.85</v>
       </c>
-      <c r="H15" s="29">
+      <c r="H15" s="27">
         <f t="shared" ref="H15" si="2">MIN(H13:H14)</f>
         <v>313.16000000000003</v>
       </c>
-      <c r="I15" s="29">
+      <c r="I15" s="27">
         <f t="shared" ref="I15" si="3">MIN(I13:I14)</f>
         <v>813.04</v>
       </c>
-      <c r="J15" s="29">
+      <c r="J15" s="27">
         <f t="shared" ref="J15" si="4">MIN(J13:J14)</f>
         <v>1611.21</v>
       </c>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
     </row>
     <row r="16" spans="2:14" s="6" customFormat="1" ht="16" thickTop="1">
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="30">
+      <c r="D16" s="28">
         <f>D$6/D15</f>
         <v>66276.501385894677</v>
       </c>
-      <c r="F16" s="30">
+      <c r="F16" s="28">
         <f t="shared" ref="F16:J16" si="5">F$6/F15</f>
         <v>37.654320987654316</v>
       </c>
-      <c r="G16" s="30">
+      <c r="G16" s="28">
         <f t="shared" si="5"/>
         <v>40.920502092050206</v>
       </c>
-      <c r="H16" s="30">
+      <c r="H16" s="28">
         <f t="shared" si="5"/>
         <v>38.411674543364413</v>
       </c>
-      <c r="I16" s="30">
+      <c r="I16" s="28">
         <f t="shared" si="5"/>
         <v>39.860277477122899</v>
       </c>
-      <c r="J16" s="30">
+      <c r="J16" s="28">
         <f t="shared" si="5"/>
         <v>41.336635199632575</v>
       </c>
-      <c r="K16" s="30"/>
-      <c r="L16" s="30"/>
-      <c r="N16" s="20"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="N16" s="19"/>
     </row>
     <row r="17" spans="2:14" s="1" customFormat="1">
       <c r="D17" s="5"/>
@@ -2356,6 +2499,7 @@
       <c r="B20" s="10" t="s">
         <v>13</v>
       </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="5"/>
       <c r="E20" s="1"/>
       <c r="F20" s="5"/>
@@ -2370,21 +2514,22 @@
       <c r="B21" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="35">
+      <c r="C21" s="34"/>
+      <c r="D21" s="32">
         <v>54.01</v>
       </c>
-      <c r="E21" s="37"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35">
+      <c r="E21" s="34"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="32">
         <v>43.67</v>
       </c>
-      <c r="H21" s="35">
+      <c r="H21" s="32">
         <v>202.11</v>
       </c>
-      <c r="I21" s="35"/>
-      <c r="J21" s="35"/>
-      <c r="K21" s="35"/>
-      <c r="L21" s="35"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
     </row>
     <row r="22" spans="2:14">
       <c r="B22" s="7" t="s">
@@ -2393,64 +2538,64 @@
       <c r="D22" s="17">
         <v>57.87</v>
       </c>
-      <c r="F22" s="17"/>
+      <c r="F22" s="4"/>
       <c r="G22" s="17">
         <v>44.08</v>
       </c>
       <c r="H22" s="17">
         <v>199.28</v>
       </c>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
     </row>
     <row r="23" spans="2:14" ht="16" thickBot="1">
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="29">
+      <c r="C23" s="33"/>
+      <c r="D23" s="27">
         <f>AVERAGE(D21:D22)</f>
         <v>55.94</v>
       </c>
-      <c r="E23" s="28"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29">
+      <c r="E23" s="33"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="27">
         <f>AVERAGE(G21:G22)</f>
         <v>43.875</v>
       </c>
-      <c r="H23" s="29">
+      <c r="H23" s="27">
         <f>AVERAGE(H21:H22)</f>
         <v>200.69499999999999</v>
       </c>
-      <c r="I23" s="29"/>
-      <c r="J23" s="29"/>
-      <c r="K23" s="29"/>
-      <c r="L23" s="29"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
     </row>
     <row r="24" spans="2:14" s="6" customFormat="1" ht="16" thickTop="1">
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="30">
+      <c r="D24" s="28">
         <f>D$6/D23</f>
         <v>38469.75330711477</v>
       </c>
-      <c r="F24" s="24"/>
-      <c r="G24" s="30">
+      <c r="F24" s="23"/>
+      <c r="G24" s="28">
         <f>G$6/G23</f>
         <v>33.435897435897438</v>
       </c>
-      <c r="H24" s="30">
+      <c r="H24" s="28">
         <f>H$6/H23</f>
         <v>59.936719898353225</v>
       </c>
-      <c r="I24" s="24"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="24"/>
-      <c r="L24" s="24"/>
-      <c r="N24" s="20"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="N24" s="19"/>
     </row>
     <row r="25" spans="2:14">
       <c r="D25" s="4"/>
@@ -2479,140 +2624,142 @@
       <c r="B27" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D27" s="35">
+      <c r="C27" s="35"/>
+      <c r="D27" s="32">
         <v>54.25</v>
       </c>
-      <c r="E27" s="38"/>
-      <c r="F27" s="35">
+      <c r="E27" s="35"/>
+      <c r="F27" s="32">
         <v>47.46</v>
       </c>
-      <c r="G27" s="35">
+      <c r="G27" s="32">
         <v>62.26</v>
       </c>
-      <c r="H27" s="35">
+      <c r="H27" s="32">
         <v>206.11</v>
       </c>
-      <c r="I27" s="35">
+      <c r="I27" s="32">
         <v>502.27</v>
       </c>
-      <c r="J27" s="35">
+      <c r="J27" s="32">
         <v>993.72</v>
       </c>
-      <c r="K27" s="35">
+      <c r="K27" s="32">
         <v>1809.66</v>
       </c>
-      <c r="L27" s="35"/>
+      <c r="L27" s="4"/>
     </row>
     <row r="28" spans="2:14">
       <c r="B28" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="35">
+      <c r="C28" s="29"/>
+      <c r="D28" s="32">
         <v>53.38</v>
       </c>
-      <c r="E28" s="31"/>
-      <c r="F28" s="35">
+      <c r="E28" s="29"/>
+      <c r="F28" s="32">
         <v>45.97</v>
       </c>
-      <c r="G28" s="35">
+      <c r="G28" s="32">
         <v>59.37</v>
       </c>
-      <c r="H28" s="35">
+      <c r="H28" s="32">
         <v>196.24</v>
       </c>
-      <c r="I28" s="35">
+      <c r="I28" s="32">
         <v>478.54</v>
       </c>
-      <c r="J28" s="35">
+      <c r="J28" s="32">
         <v>901.08</v>
       </c>
-      <c r="K28" s="35">
+      <c r="K28" s="32">
         <v>1681.88</v>
       </c>
-      <c r="L28" s="35"/>
+      <c r="L28" s="4"/>
     </row>
     <row r="29" spans="2:14" ht="16" thickBot="1">
-      <c r="B29" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="C29" s="28"/>
-      <c r="D29" s="29">
+      <c r="B29" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="33"/>
+      <c r="D29" s="27">
         <f>MIN(D27:D28)</f>
         <v>53.38</v>
       </c>
-      <c r="E29" s="28"/>
-      <c r="F29" s="29">
+      <c r="E29" s="33"/>
+      <c r="F29" s="27">
         <f t="shared" ref="F29" si="6">MIN(F27:F28)</f>
         <v>45.97</v>
       </c>
-      <c r="G29" s="29">
+      <c r="G29" s="27">
         <f t="shared" ref="G29" si="7">MIN(G27:G28)</f>
         <v>59.37</v>
       </c>
-      <c r="H29" s="29">
+      <c r="H29" s="27">
         <f t="shared" ref="H29" si="8">MIN(H27:H28)</f>
         <v>196.24</v>
       </c>
-      <c r="I29" s="29">
+      <c r="I29" s="27">
         <f t="shared" ref="I29" si="9">MIN(I27:I28)</f>
         <v>478.54</v>
       </c>
-      <c r="J29" s="29">
+      <c r="J29" s="27">
         <f t="shared" ref="J29" si="10">MIN(J27:J28)</f>
         <v>901.08</v>
       </c>
-      <c r="K29" s="29">
+      <c r="K29" s="27">
         <f t="shared" ref="K29" si="11">MIN(K27:K28)</f>
         <v>1681.88</v>
       </c>
-      <c r="L29" s="29"/>
+      <c r="L29" s="4"/>
     </row>
     <row r="30" spans="2:14" s="6" customFormat="1" ht="16" thickTop="1">
-      <c r="B30" s="23" t="s">
+      <c r="B30" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="D30" s="30">
+      <c r="D30" s="28">
         <f>D$6/D29</f>
         <v>40314.687148744844</v>
       </c>
-      <c r="F30" s="40">
+      <c r="F30" s="30">
         <f t="shared" ref="F30:K30" si="12">F$6/F29</f>
         <v>3.9808570807048076</v>
       </c>
-      <c r="G30" s="40">
+      <c r="G30" s="30">
         <f t="shared" si="12"/>
         <v>24.70944921677615</v>
       </c>
-      <c r="H30" s="40">
+      <c r="H30" s="30">
         <f t="shared" si="12"/>
         <v>61.297390949857316</v>
       </c>
-      <c r="I30" s="40">
+      <c r="I30" s="30">
         <f t="shared" si="12"/>
         <v>67.722656413256985</v>
       </c>
-      <c r="J30" s="40">
+      <c r="J30" s="30">
         <f t="shared" si="12"/>
         <v>73.913525991032984</v>
       </c>
-      <c r="K30" s="40">
+      <c r="K30" s="30">
         <f t="shared" si="12"/>
         <v>78.091183675410846</v>
       </c>
-      <c r="L30" s="30"/>
-      <c r="N30" s="20"/>
+      <c r="L30" s="4"/>
+      <c r="N30" s="19"/>
     </row>
     <row r="31" spans="2:14" s="6" customFormat="1">
-      <c r="B31" s="23"/>
-      <c r="D31" s="30"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="30"/>
-      <c r="H31" s="30"/>
-      <c r="I31" s="30"/>
-      <c r="J31" s="30"/>
-      <c r="K31" s="30"/>
-      <c r="L31" s="30"/>
-      <c r="N31" s="20"/>
+      <c r="B31" s="22"/>
+      <c r="D31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="28"/>
+      <c r="J31" s="28"/>
+      <c r="K31" s="28"/>
+      <c r="L31" s="28"/>
+      <c r="N31" s="19"/>
     </row>
     <row r="32" spans="2:14">
       <c r="B32" s="14" t="s">
@@ -2627,459 +2774,421 @@
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
     </row>
-    <row r="33" spans="2:14">
-      <c r="B33" s="18" t="s">
+    <row r="33" spans="1:14">
+      <c r="B33" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="34">
+      <c r="C33" s="40"/>
+      <c r="D33" s="39">
         <v>46.16</v>
       </c>
-      <c r="E33" s="39"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="34"/>
-      <c r="H33" s="34">
+      <c r="E33" s="40"/>
+      <c r="F33" s="39"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="39">
         <v>119.35</v>
       </c>
-      <c r="I33" s="34"/>
-      <c r="J33" s="34"/>
-      <c r="K33" s="34"/>
-      <c r="L33" s="34"/>
-    </row>
-    <row r="34" spans="2:14">
-      <c r="B34" s="21" t="s">
+      <c r="I33" s="39"/>
+      <c r="J33" s="39"/>
+      <c r="K33" s="39"/>
+      <c r="L33" s="39"/>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="B34" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="32">
+      <c r="C34" s="38"/>
+      <c r="D34" s="42">
         <f>D$6/D33</f>
         <v>46620.407279029467</v>
       </c>
-      <c r="E34" s="13"/>
-      <c r="F34" s="32" t="e">
-        <f t="shared" ref="F34:K34" si="13">F$6/F33</f>
+      <c r="E34" s="38"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="42"/>
+      <c r="H34" s="43">
+        <f t="shared" ref="H34" si="13">H$6/H33</f>
+        <v>100.78759949727691</v>
+      </c>
+      <c r="I34" s="42"/>
+      <c r="J34" s="42"/>
+      <c r="K34" s="42"/>
+      <c r="L34" s="42"/>
+    </row>
+    <row r="35" spans="1:14" s="6" customFormat="1">
+      <c r="B35" s="22"/>
+      <c r="D35" s="28"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="28"/>
+      <c r="I35" s="28"/>
+      <c r="J35" s="28"/>
+      <c r="K35" s="28"/>
+      <c r="L35" s="28"/>
+      <c r="N35" s="19"/>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="B36" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" s="40"/>
+      <c r="D36" s="39"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="39"/>
+      <c r="G36" s="39"/>
+      <c r="H36" s="39">
+        <v>123.64</v>
+      </c>
+      <c r="I36" s="39"/>
+      <c r="J36" s="39"/>
+      <c r="K36" s="39"/>
+      <c r="L36" s="39"/>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="B37" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" s="38"/>
+      <c r="D37" s="42" t="e">
+        <f>D$6/D36</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G34" s="32" t="e">
-        <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H34" s="25">
-        <f t="shared" si="13"/>
-        <v>100.78759949727691</v>
-      </c>
-      <c r="I34" s="32" t="e">
-        <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J34" s="32" t="e">
-        <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K34" s="32" t="e">
-        <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L34" s="32"/>
-    </row>
-    <row r="35" spans="2:14">
-      <c r="B35" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="34"/>
-      <c r="E35" s="39"/>
-      <c r="F35" s="34"/>
-      <c r="G35" s="34"/>
-      <c r="H35" s="34">
-        <v>123.64</v>
-      </c>
-      <c r="I35" s="34"/>
-      <c r="J35" s="34"/>
-      <c r="K35" s="34"/>
-      <c r="L35" s="34"/>
-    </row>
-    <row r="36" spans="2:14">
-      <c r="B36" s="21" t="s">
+      <c r="E37" s="38"/>
+      <c r="F37" s="42"/>
+      <c r="G37" s="42"/>
+      <c r="H37" s="43">
+        <f t="shared" ref="H37" si="14">H$6/H36</f>
+        <v>97.290520867033322</v>
+      </c>
+      <c r="I37" s="42"/>
+      <c r="J37" s="42"/>
+      <c r="K37" s="42"/>
+      <c r="L37" s="42"/>
+    </row>
+    <row r="38" spans="1:14" s="6" customFormat="1">
+      <c r="B38" s="22"/>
+      <c r="D38" s="28"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="28"/>
+      <c r="I38" s="28"/>
+      <c r="J38" s="28"/>
+      <c r="K38" s="28"/>
+      <c r="L38" s="44"/>
+      <c r="N38" s="19"/>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="B39" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" s="36"/>
+      <c r="D39" s="31">
+        <v>38.659999999999997</v>
+      </c>
+      <c r="E39" s="36"/>
+      <c r="F39" s="31">
+        <v>20.48</v>
+      </c>
+      <c r="G39" s="31">
+        <v>27.92</v>
+      </c>
+      <c r="H39" s="31">
+        <v>70.45</v>
+      </c>
+      <c r="I39" s="31">
+        <v>142.12</v>
+      </c>
+      <c r="J39" s="31">
+        <v>259.08999999999997</v>
+      </c>
+      <c r="K39" s="31">
+        <v>476.05</v>
+      </c>
+      <c r="L39" s="45" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" s="6" customFormat="1">
+      <c r="B40" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="32" t="e">
-        <f>D$6/D35</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E36" s="13"/>
-      <c r="F36" s="32" t="e">
-        <f t="shared" ref="F36:K36" si="14">F$6/F35</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G36" s="32" t="e">
-        <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H36" s="25">
-        <f t="shared" si="14"/>
-        <v>97.290520867033322</v>
-      </c>
-      <c r="I36" s="32" t="e">
-        <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J36" s="32" t="e">
-        <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K36" s="32" t="e">
-        <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L36" s="32"/>
-    </row>
-    <row r="37" spans="2:14">
-      <c r="B37" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="34">
-        <v>38.659999999999997</v>
-      </c>
-      <c r="E37" s="39"/>
-      <c r="F37" s="34">
-        <v>20.48</v>
-      </c>
-      <c r="G37" s="34">
-        <v>27.92</v>
-      </c>
-      <c r="H37" s="34">
-        <v>70.45</v>
-      </c>
-      <c r="I37" s="34">
-        <v>142.12</v>
-      </c>
-      <c r="J37" s="34">
-        <v>259.08999999999997</v>
-      </c>
-      <c r="K37" s="34">
-        <v>476.05</v>
-      </c>
-      <c r="L37" s="34"/>
-    </row>
-    <row r="38" spans="2:14" s="6" customFormat="1">
-      <c r="B38" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C38" s="19"/>
-      <c r="D38" s="25">
-        <f>D$6/D37</f>
+      <c r="C40" s="25"/>
+      <c r="D40" s="24">
+        <f>D$6/D39</f>
         <v>55664.718054837045</v>
       </c>
-      <c r="E38" s="26"/>
-      <c r="F38" s="40">
-        <f t="shared" ref="F38:L38" si="15">F$6/F37</f>
+      <c r="E40" s="25"/>
+      <c r="F40" s="30">
+        <f t="shared" ref="F40:K40" si="15">F$6/F39</f>
         <v>8.935546875</v>
       </c>
-      <c r="G38" s="40">
+      <c r="G40" s="30">
         <f t="shared" si="15"/>
         <v>52.542979942693407</v>
       </c>
-      <c r="H38" s="41">
+      <c r="H40" s="30">
         <f t="shared" si="15"/>
         <v>170.74520936834634</v>
       </c>
-      <c r="I38" s="41">
+      <c r="I40" s="30">
         <f t="shared" si="15"/>
         <v>228.03264846608499</v>
       </c>
-      <c r="J38" s="41">
+      <c r="J40" s="30">
         <f t="shared" si="15"/>
         <v>257.06125284650125</v>
       </c>
-      <c r="K38" s="40">
+      <c r="K40" s="30">
         <f t="shared" si="15"/>
         <v>275.89538913979624</v>
       </c>
-      <c r="L38" s="40" t="e">
-        <f t="shared" si="15"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N38" s="20"/>
-    </row>
-    <row r="39" spans="2:14">
-      <c r="B39" s="18" t="s">
+      <c r="L40" s="44"/>
+      <c r="N40" s="19"/>
+    </row>
+    <row r="41" spans="1:14" s="6" customFormat="1">
+      <c r="B41" s="22"/>
+      <c r="D41" s="28"/>
+      <c r="F41" s="28"/>
+      <c r="G41" s="28"/>
+      <c r="H41" s="28"/>
+      <c r="I41" s="28"/>
+      <c r="J41" s="28"/>
+      <c r="K41" s="28"/>
+      <c r="L41" s="44"/>
+      <c r="N41" s="19"/>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="B42" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C39" s="13"/>
-      <c r="D39" s="34">
+      <c r="C42" s="36"/>
+      <c r="D42" s="31">
         <v>37.700000000000003</v>
       </c>
-      <c r="E39" s="39"/>
-      <c r="F39" s="34">
+      <c r="E42" s="36"/>
+      <c r="F42" s="31">
         <v>24.17</v>
       </c>
-      <c r="G39" s="34">
+      <c r="G42" s="31">
         <v>43.78</v>
       </c>
-      <c r="H39" s="34">
+      <c r="H42" s="31">
         <v>79.19</v>
       </c>
-      <c r="I39" s="34">
+      <c r="I42" s="31">
         <v>149.87</v>
       </c>
-      <c r="J39" s="34">
+      <c r="J42" s="31">
         <v>263.93</v>
       </c>
-      <c r="K39" s="34">
+      <c r="K42" s="31">
         <v>474.26</v>
       </c>
-      <c r="L39" s="34" t="s">
+      <c r="L42" s="45" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="2:14">
-      <c r="B40" s="21" t="s">
+    <row r="43" spans="1:14">
+      <c r="A43" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C40" s="13"/>
-      <c r="D40" s="32">
-        <f>D$6/D39</f>
+      <c r="C43" s="13"/>
+      <c r="D43" s="30">
+        <f>D$6/D42</f>
         <v>57082.175066312993</v>
       </c>
-      <c r="E40" s="13"/>
-      <c r="F40" s="32">
-        <f t="shared" ref="F40:K40" si="16">F$6/F39</f>
+      <c r="E43" s="13"/>
+      <c r="F43" s="30">
+        <f t="shared" ref="F43:K43" si="16">F$6/F42</f>
         <v>7.5713694662805127</v>
       </c>
-      <c r="G40" s="32">
+      <c r="G43" s="30">
         <f t="shared" si="16"/>
         <v>33.508451347647323</v>
       </c>
-      <c r="H40" s="25">
+      <c r="H43" s="24">
         <f t="shared" si="16"/>
         <v>151.90049248642507</v>
       </c>
-      <c r="I40" s="25">
+      <c r="I43" s="24">
         <f t="shared" si="16"/>
         <v>216.24074197637952</v>
       </c>
-      <c r="J40" s="25">
+      <c r="J43" s="24">
         <f t="shared" si="16"/>
         <v>252.34721327624749</v>
       </c>
-      <c r="K40" s="32">
+      <c r="K43" s="30">
         <f t="shared" si="16"/>
         <v>276.93670138742465</v>
       </c>
-      <c r="L40" s="32"/>
-    </row>
-    <row r="41" spans="2:14">
-      <c r="B41" s="18" t="s">
+      <c r="L43" s="44"/>
+    </row>
+    <row r="44" spans="1:14" s="6" customFormat="1">
+      <c r="B44" s="22"/>
+      <c r="D44" s="28"/>
+      <c r="F44" s="28"/>
+      <c r="G44" s="28"/>
+      <c r="H44" s="28"/>
+      <c r="I44" s="28"/>
+      <c r="J44" s="28"/>
+      <c r="K44" s="28"/>
+      <c r="L44" s="28"/>
+      <c r="N44" s="19"/>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="B45" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C41" s="13"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="34"/>
-      <c r="G41" s="34"/>
-      <c r="H41" s="34"/>
-      <c r="I41" s="34"/>
-      <c r="J41" s="34"/>
-      <c r="K41" s="34"/>
-      <c r="L41" s="34"/>
-    </row>
-    <row r="42" spans="2:14">
-      <c r="B42" s="21" t="s">
+      <c r="C45" s="13"/>
+      <c r="D45" s="16">
+        <v>34.86</v>
+      </c>
+      <c r="E45" s="13"/>
+      <c r="F45" s="31">
+        <v>22.86</v>
+      </c>
+      <c r="G45" s="31">
+        <v>36.79</v>
+      </c>
+      <c r="H45" s="31">
+        <v>56.29</v>
+      </c>
+      <c r="I45" s="31">
+        <v>98.95</v>
+      </c>
+      <c r="J45" s="31">
+        <v>146.63999999999999</v>
+      </c>
+      <c r="K45" s="31">
+        <v>255.54</v>
+      </c>
+      <c r="L45" s="31">
+        <v>2152</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="B46" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="32" t="e">
-        <f>D$6/D41</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E42" s="13"/>
-      <c r="F42" s="32" t="e">
-        <f t="shared" ref="F42:K42" si="17">F$6/F41</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G42" s="32" t="e">
+      <c r="C46" s="13"/>
+      <c r="D46" s="30">
+        <f>D$6/D45</f>
+        <v>61732.587492828461</v>
+      </c>
+      <c r="E46" s="13"/>
+      <c r="F46" s="30">
+        <f t="shared" ref="F46:L46" si="17">F$6/F45</f>
+        <v>8.0052493438320216</v>
+      </c>
+      <c r="G46" s="30">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H42" s="32" t="e">
+        <v>39.874966023375919</v>
+      </c>
+      <c r="H46" s="30">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I42" s="32" t="e">
+        <v>213.69692662995203</v>
+      </c>
+      <c r="I46" s="30">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J42" s="32" t="e">
+        <v>327.5189489641233</v>
+      </c>
+      <c r="J46" s="30">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K42" s="32" t="e">
+        <v>454.18712493180584</v>
+      </c>
+      <c r="K46" s="30">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L42" s="32"/>
-    </row>
-    <row r="43" spans="2:14">
-      <c r="B43" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C43" s="13"/>
-      <c r="D43" s="16">
-        <v>34.86</v>
-      </c>
-      <c r="E43" s="13"/>
-      <c r="F43" s="34">
-        <v>22.86</v>
-      </c>
-      <c r="G43" s="34">
-        <v>36.79</v>
-      </c>
-      <c r="H43" s="34">
-        <v>56.29</v>
-      </c>
-      <c r="I43" s="34">
-        <v>98.95</v>
-      </c>
-      <c r="J43" s="34">
-        <v>146.63999999999999</v>
-      </c>
-      <c r="K43" s="34">
-        <v>255.54</v>
-      </c>
-      <c r="L43" s="34">
-        <v>2152</v>
-      </c>
-    </row>
-    <row r="44" spans="2:14">
-      <c r="B44" s="21" t="s">
+        <v>513.97041559051422</v>
+      </c>
+      <c r="L46" s="30">
+        <f t="shared" si="17"/>
+        <v>584.59526022304829</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" s="6" customFormat="1">
+      <c r="B47" s="22"/>
+      <c r="D47" s="28"/>
+      <c r="F47" s="28"/>
+      <c r="G47" s="28"/>
+      <c r="H47" s="28"/>
+      <c r="I47" s="28"/>
+      <c r="J47" s="28"/>
+      <c r="K47" s="28"/>
+      <c r="L47" s="28"/>
+      <c r="N47" s="19"/>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="B48" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C48" s="13"/>
+      <c r="D48" s="16">
+        <v>35.630000000000003</v>
+      </c>
+      <c r="E48" s="13"/>
+      <c r="F48" s="31">
+        <v>19.68</v>
+      </c>
+      <c r="G48" s="31">
+        <v>40.36</v>
+      </c>
+      <c r="H48" s="31">
+        <v>50.71</v>
+      </c>
+      <c r="I48" s="31">
+        <v>70.760000000000005</v>
+      </c>
+      <c r="J48" s="31">
+        <v>99.87</v>
+      </c>
+      <c r="K48" s="31">
+        <v>161.82</v>
+      </c>
+      <c r="L48" s="31">
+        <v>1106.28</v>
+      </c>
+    </row>
+    <row r="49" spans="2:14">
+      <c r="B49" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C44" s="13"/>
-      <c r="D44" s="32">
-        <f>D$6/D43</f>
-        <v>61732.587492828461</v>
-      </c>
-      <c r="E44" s="13"/>
-      <c r="F44" s="40">
-        <f t="shared" ref="F44:L44" si="18">F$6/F43</f>
-        <v>8.0052493438320216</v>
-      </c>
-      <c r="G44" s="40">
+      <c r="C49" s="13"/>
+      <c r="D49" s="30">
+        <f>D$6/D48</f>
+        <v>60398.484423238842</v>
+      </c>
+      <c r="E49" s="13"/>
+      <c r="F49" s="30">
+        <f t="shared" ref="F49:L49" si="18">F$6/F48</f>
+        <v>9.2987804878048781</v>
+      </c>
+      <c r="G49" s="30">
         <f t="shared" si="18"/>
-        <v>39.874966023375919</v>
-      </c>
-      <c r="H44" s="40">
+        <v>36.347869177403368</v>
+      </c>
+      <c r="H49" s="30">
         <f t="shared" si="18"/>
-        <v>213.69692662995203</v>
-      </c>
-      <c r="I44" s="40">
+        <v>237.21159534608557</v>
+      </c>
+      <c r="I49" s="30">
         <f t="shared" si="18"/>
-        <v>327.5189489641233</v>
-      </c>
-      <c r="J44" s="40">
+        <v>457.99886941775009</v>
+      </c>
+      <c r="J49" s="30">
         <f t="shared" si="18"/>
-        <v>454.18712493180584</v>
-      </c>
-      <c r="K44" s="40">
+        <v>666.88695303895065</v>
+      </c>
+      <c r="K49" s="30">
         <f t="shared" si="18"/>
-        <v>513.97041559051422</v>
-      </c>
-      <c r="L44" s="40">
+        <v>811.64256581386735</v>
+      </c>
+      <c r="L49" s="30">
         <f t="shared" si="18"/>
-        <v>584.59526022304829</v>
-      </c>
-    </row>
-    <row r="45" spans="2:14">
-      <c r="B45" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="C45" s="13"/>
-      <c r="D45" s="16"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="34"/>
-      <c r="G45" s="34"/>
-      <c r="H45" s="34"/>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
-      <c r="K45" s="34"/>
-      <c r="L45" s="34"/>
-    </row>
-    <row r="46" spans="2:14">
-      <c r="B46" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C46" s="13"/>
-      <c r="D46" s="32" t="e">
-        <f>D$6/D45</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E46" s="13"/>
-      <c r="F46" s="32" t="e">
-        <f t="shared" ref="F46:K46" si="19">F$6/F45</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G46" s="32" t="e">
-        <f t="shared" si="19"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H46" s="32" t="e">
-        <f t="shared" si="19"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I46" s="32" t="e">
-        <f t="shared" si="19"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J46" s="32" t="e">
-        <f t="shared" si="19"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K46" s="32" t="e">
-        <f t="shared" si="19"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L46" s="32"/>
-    </row>
-    <row r="47" spans="2:14">
-      <c r="D47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
-      <c r="I47" s="4"/>
-      <c r="J47" s="4"/>
-      <c r="K47" s="4"/>
-      <c r="L47" s="4"/>
-    </row>
-    <row r="48" spans="2:14">
-      <c r="B48" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9"/>
-      <c r="H48" s="9"/>
-      <c r="I48" s="9"/>
-      <c r="J48" s="9"/>
-      <c r="K48" s="9"/>
-      <c r="L48" s="9"/>
-    </row>
-    <row r="49" spans="2:14" s="1" customFormat="1">
-      <c r="B49" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
-      <c r="H49" s="5"/>
-      <c r="I49" s="5"/>
-      <c r="J49" s="5"/>
-      <c r="K49" s="5"/>
-      <c r="L49" s="5"/>
+        <v>1137.1885960154752</v>
+      </c>
     </row>
     <row r="50" spans="2:14">
       <c r="D50" s="4"/>
@@ -3093,7 +3202,7 @@
     </row>
     <row r="51" spans="2:14">
       <c r="B51" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C51" s="9"/>
       <c r="D51" s="9"/>
@@ -3107,6 +3216,9 @@
       <c r="L51" s="9"/>
     </row>
     <row r="52" spans="2:14" s="1" customFormat="1">
+      <c r="B52" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="D52" s="5"/>
       <c r="F52" s="5"/>
       <c r="G52" s="5"/>
@@ -3116,576 +3228,670 @@
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
     </row>
-    <row r="53" spans="2:14" s="11" customFormat="1">
-      <c r="B53" s="10" t="s">
+    <row r="53" spans="2:14">
+      <c r="D53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="4"/>
+      <c r="L53" s="4"/>
+    </row>
+    <row r="54" spans="2:14">
+      <c r="B54" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
+      <c r="H54" s="9"/>
+      <c r="I54" s="9"/>
+      <c r="J54" s="9"/>
+      <c r="K54" s="9"/>
+      <c r="L54" s="9"/>
+    </row>
+    <row r="55" spans="2:14" s="1" customFormat="1">
+      <c r="D55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="5"/>
+      <c r="J55" s="5"/>
+      <c r="K55" s="5"/>
+      <c r="L55" s="5"/>
+    </row>
+    <row r="56" spans="2:14" s="11" customFormat="1">
+      <c r="B56" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D53" s="5"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5"/>
-      <c r="H53" s="5"/>
-      <c r="I53" s="5"/>
-      <c r="J53" s="5"/>
-      <c r="K53" s="5"/>
-      <c r="L53" s="5"/>
-    </row>
-    <row r="54" spans="2:14">
-      <c r="B54" s="22" t="s">
+      <c r="D56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="5"/>
+      <c r="J56" s="5"/>
+      <c r="K56" s="5"/>
+      <c r="L56" s="5"/>
+    </row>
+    <row r="57" spans="2:14">
+      <c r="B57" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D54" s="35">
+      <c r="C57" s="34"/>
+      <c r="D57" s="32">
         <v>56</v>
       </c>
-      <c r="E54" s="37"/>
-      <c r="F54" s="35"/>
-      <c r="G54" s="35">
+      <c r="E57" s="34"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="32">
         <v>373.94</v>
       </c>
-      <c r="H54" s="35">
+      <c r="H57" s="32">
         <v>1009.81</v>
       </c>
-      <c r="I54" s="35"/>
-      <c r="J54" s="35"/>
-      <c r="K54" s="35"/>
-      <c r="L54" s="35"/>
-    </row>
-    <row r="55" spans="2:14" s="6" customFormat="1">
-      <c r="B55" s="23" t="s">
+      <c r="I57" s="5"/>
+      <c r="J57" s="5"/>
+      <c r="K57" s="5"/>
+      <c r="L57" s="5"/>
+    </row>
+    <row r="58" spans="2:14" s="6" customFormat="1">
+      <c r="B58" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="D55" s="32">
-        <f>D$6/D54</f>
+      <c r="D58" s="30">
+        <f>D$6/D57</f>
         <v>38428.535714285717</v>
       </c>
-      <c r="F55" s="33"/>
-      <c r="G55" s="32">
-        <f>G$6/G54</f>
+      <c r="F58" s="5"/>
+      <c r="G58" s="30">
+        <f>G$6/G57</f>
         <v>3.923089265657592</v>
       </c>
-      <c r="H55" s="32">
-        <f>H$6/H54</f>
+      <c r="H58" s="30">
+        <f>H$6/H57</f>
         <v>11.912141888077956</v>
       </c>
-      <c r="I55" s="33"/>
-      <c r="J55" s="33"/>
-      <c r="K55" s="33"/>
-      <c r="L55" s="33"/>
-      <c r="N55" s="20"/>
-    </row>
-    <row r="56" spans="2:14">
-      <c r="D56" s="4"/>
-      <c r="F56" s="4"/>
-      <c r="G56" s="4"/>
-      <c r="H56" s="4"/>
-      <c r="I56" s="4"/>
-      <c r="J56" s="4"/>
-      <c r="K56" s="4"/>
-      <c r="L56" s="4"/>
-    </row>
-    <row r="57" spans="2:14">
-      <c r="B57" s="10" t="s">
+      <c r="I58" s="5"/>
+      <c r="J58" s="5"/>
+      <c r="K58" s="5"/>
+      <c r="L58" s="5"/>
+      <c r="N58" s="19"/>
+    </row>
+    <row r="59" spans="2:14">
+      <c r="D59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="4"/>
+      <c r="J59" s="4"/>
+      <c r="K59" s="4"/>
+      <c r="L59" s="4"/>
+    </row>
+    <row r="60" spans="2:14">
+      <c r="B60" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D57" s="4"/>
-      <c r="F57" s="4"/>
-      <c r="G57" s="4"/>
-      <c r="H57" s="4"/>
-      <c r="I57" s="4"/>
-      <c r="J57" s="4"/>
-      <c r="K57" s="4"/>
-      <c r="L57" s="4"/>
-    </row>
-    <row r="58" spans="2:14">
-      <c r="B58" s="7" t="s">
+      <c r="D60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
+      <c r="J60" s="4"/>
+      <c r="K60" s="4"/>
+      <c r="L60" s="4"/>
+    </row>
+    <row r="61" spans="2:14">
+      <c r="B61" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D58" s="35">
+      <c r="C61" s="35"/>
+      <c r="D61" s="32">
         <v>52.59</v>
       </c>
-      <c r="E58" s="38"/>
-      <c r="F58" s="35">
+      <c r="E61" s="35"/>
+      <c r="F61" s="32">
         <v>87.07</v>
       </c>
-      <c r="G58" s="35">
+      <c r="G61" s="32">
         <v>141.15</v>
       </c>
-      <c r="H58" s="35">
+      <c r="H61" s="32">
         <v>374.87</v>
       </c>
-      <c r="I58" s="35">
+      <c r="I61" s="32">
         <v>832.1</v>
       </c>
-      <c r="J58" s="35">
+      <c r="J61" s="32">
         <v>1536.44</v>
       </c>
-      <c r="K58" s="35" t="s">
+      <c r="K61" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="L58" s="35"/>
-    </row>
-    <row r="59" spans="2:14">
-      <c r="B59" s="7" t="s">
+      <c r="L61" s="4"/>
+    </row>
+    <row r="62" spans="2:14">
+      <c r="B62" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D59" s="35">
+      <c r="C62" s="29"/>
+      <c r="D62" s="32">
         <v>52.92</v>
       </c>
-      <c r="E59" s="31"/>
-      <c r="F59" s="35">
+      <c r="E62" s="29"/>
+      <c r="F62" s="32">
         <v>78.75</v>
       </c>
-      <c r="G59" s="35">
+      <c r="G62" s="32">
         <v>137.38999999999999</v>
       </c>
-      <c r="H59" s="35">
+      <c r="H62" s="32">
         <v>367.1</v>
       </c>
-      <c r="I59" s="35">
+      <c r="I62" s="32">
         <v>769.77</v>
       </c>
-      <c r="J59" s="35">
+      <c r="J62" s="32">
         <v>1418.92</v>
       </c>
-      <c r="K59" s="35" t="s">
+      <c r="K62" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="L59" s="35"/>
-    </row>
-    <row r="60" spans="2:14" ht="16" thickBot="1">
-      <c r="B60" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="C60" s="28"/>
-      <c r="D60" s="29">
-        <f>MIN(D58:D59)</f>
+      <c r="L62" s="4"/>
+    </row>
+    <row r="63" spans="2:14" ht="16" thickBot="1">
+      <c r="B63" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C63" s="33"/>
+      <c r="D63" s="27">
+        <f>MIN(D61:D62)</f>
         <v>52.59</v>
       </c>
-      <c r="E60" s="28"/>
-      <c r="F60" s="29">
-        <f t="shared" ref="F60:J60" si="20">MIN(F58:F59)</f>
+      <c r="E63" s="33"/>
+      <c r="F63" s="27">
+        <f t="shared" ref="F63:J63" si="19">MIN(F61:F62)</f>
         <v>78.75</v>
       </c>
-      <c r="G60" s="29">
+      <c r="G63" s="27">
+        <f t="shared" si="19"/>
+        <v>137.38999999999999</v>
+      </c>
+      <c r="H63" s="27">
+        <f t="shared" si="19"/>
+        <v>367.1</v>
+      </c>
+      <c r="I63" s="27">
+        <f t="shared" si="19"/>
+        <v>769.77</v>
+      </c>
+      <c r="J63" s="27">
+        <f t="shared" si="19"/>
+        <v>1418.92</v>
+      </c>
+      <c r="K63" s="27"/>
+      <c r="L63" s="4"/>
+    </row>
+    <row r="64" spans="2:14" s="6" customFormat="1" ht="16" thickTop="1">
+      <c r="B64" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D64" s="28">
+        <f>D$6/D63</f>
+        <v>40920.28902833238</v>
+      </c>
+      <c r="F64" s="28">
+        <f t="shared" ref="F64:J64" si="20">F$6/F63</f>
+        <v>2.323809523809524</v>
+      </c>
+      <c r="G64" s="28">
         <f t="shared" si="20"/>
-        <v>137.38999999999999</v>
-      </c>
-      <c r="H60" s="29">
+        <v>10.677633015503313</v>
+      </c>
+      <c r="H64" s="28">
         <f t="shared" si="20"/>
-        <v>367.1</v>
-      </c>
-      <c r="I60" s="29">
+        <v>32.767638245709612</v>
+      </c>
+      <c r="I64" s="28">
         <f t="shared" si="20"/>
-        <v>769.77</v>
-      </c>
-      <c r="J60" s="29">
+        <v>42.100887278018114</v>
+      </c>
+      <c r="J64" s="28">
         <f t="shared" si="20"/>
-        <v>1418.92</v>
-      </c>
-      <c r="K60" s="29"/>
-      <c r="L60" s="29"/>
-    </row>
-    <row r="61" spans="2:14" s="6" customFormat="1" ht="16" thickTop="1">
-      <c r="B61" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="D61" s="30">
-        <f>D$6/D60</f>
-        <v>40920.28902833238</v>
-      </c>
-      <c r="F61" s="30">
-        <f t="shared" ref="F61:J61" si="21">F$6/F60</f>
-        <v>2.323809523809524</v>
-      </c>
-      <c r="G61" s="30">
+        <v>46.938516618273049</v>
+      </c>
+      <c r="K64" s="28"/>
+      <c r="L64" s="28"/>
+      <c r="N64" s="19"/>
+    </row>
+    <row r="65" spans="2:14" s="6" customFormat="1">
+      <c r="B65" s="22"/>
+      <c r="D65" s="28"/>
+      <c r="F65" s="28"/>
+      <c r="G65" s="28"/>
+      <c r="H65" s="28"/>
+      <c r="I65" s="28"/>
+      <c r="J65" s="28"/>
+      <c r="K65" s="28"/>
+      <c r="L65" s="28"/>
+      <c r="N65" s="19"/>
+    </row>
+    <row r="66" spans="2:14">
+      <c r="B66" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D66" s="4"/>
+      <c r="F66" s="4"/>
+      <c r="G66" s="4"/>
+      <c r="H66" s="4"/>
+      <c r="I66" s="4"/>
+      <c r="J66" s="4"/>
+      <c r="K66" s="4"/>
+      <c r="L66" s="4"/>
+    </row>
+    <row r="67" spans="2:14">
+      <c r="B67" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="C67" s="40"/>
+      <c r="D67" s="39">
+        <v>44.71</v>
+      </c>
+      <c r="E67" s="40"/>
+      <c r="F67" s="39"/>
+      <c r="G67" s="39"/>
+      <c r="H67" s="39">
+        <v>270.17</v>
+      </c>
+      <c r="I67" s="39"/>
+      <c r="J67" s="39"/>
+      <c r="K67" s="39"/>
+      <c r="L67" s="39"/>
+    </row>
+    <row r="68" spans="2:14">
+      <c r="B68" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="C68" s="38"/>
+      <c r="D68" s="42">
+        <f>D$6/D67</f>
+        <v>48132.364124356965</v>
+      </c>
+      <c r="E68" s="38"/>
+      <c r="F68" s="42"/>
+      <c r="G68" s="42"/>
+      <c r="H68" s="43">
+        <f>H$6/H67</f>
+        <v>44.523818336602879</v>
+      </c>
+      <c r="I68" s="42"/>
+      <c r="J68" s="42"/>
+      <c r="K68" s="42"/>
+      <c r="L68" s="42"/>
+    </row>
+    <row r="69" spans="2:14" s="6" customFormat="1">
+      <c r="B69" s="22"/>
+      <c r="D69" s="28"/>
+      <c r="F69" s="28"/>
+      <c r="G69" s="28"/>
+      <c r="H69" s="28"/>
+      <c r="I69" s="28"/>
+      <c r="J69" s="28"/>
+      <c r="K69" s="28"/>
+      <c r="L69" s="28"/>
+      <c r="N69" s="19"/>
+    </row>
+    <row r="70" spans="2:14">
+      <c r="B70" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="C70" s="40"/>
+      <c r="D70" s="39">
+        <v>43.34</v>
+      </c>
+      <c r="E70" s="40"/>
+      <c r="F70" s="39">
+        <v>117.96</v>
+      </c>
+      <c r="G70" s="39">
+        <v>248.14</v>
+      </c>
+      <c r="H70" s="39">
+        <v>433.07</v>
+      </c>
+      <c r="I70" s="39"/>
+      <c r="J70" s="39"/>
+      <c r="K70" s="39"/>
+      <c r="L70" s="39"/>
+    </row>
+    <row r="71" spans="2:14">
+      <c r="B71" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="C71" s="38"/>
+      <c r="D71" s="42">
+        <f t="shared" ref="D71:H71" si="21">D$6/D70</f>
+        <v>49653.853253345638</v>
+      </c>
+      <c r="E71" s="38"/>
+      <c r="F71" s="42">
         <f t="shared" si="21"/>
-        <v>10.677633015503313</v>
-      </c>
-      <c r="H61" s="30">
+        <v>1.5513733468972535</v>
+      </c>
+      <c r="G71" s="42">
         <f t="shared" si="21"/>
-        <v>32.767638245709612</v>
-      </c>
-      <c r="I61" s="30">
+        <v>5.9119851696622874</v>
+      </c>
+      <c r="H71" s="43">
         <f t="shared" si="21"/>
-        <v>42.100887278018114</v>
-      </c>
-      <c r="J61" s="30">
-        <f t="shared" si="21"/>
-        <v>46.938516618273049</v>
-      </c>
-      <c r="K61" s="30"/>
-      <c r="L61" s="30"/>
-      <c r="N61" s="20"/>
-    </row>
-    <row r="62" spans="2:14" s="6" customFormat="1">
-      <c r="B62" s="23"/>
-      <c r="D62" s="30"/>
-      <c r="F62" s="30"/>
-      <c r="G62" s="30"/>
-      <c r="H62" s="30"/>
-      <c r="I62" s="30"/>
-      <c r="J62" s="30"/>
-      <c r="K62" s="30"/>
-      <c r="L62" s="30"/>
-      <c r="N62" s="20"/>
-    </row>
-    <row r="63" spans="2:14">
-      <c r="B63" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D63" s="4"/>
-      <c r="F63" s="4"/>
-      <c r="G63" s="4"/>
-      <c r="H63" s="4"/>
-      <c r="I63" s="4"/>
-      <c r="J63" s="4"/>
-      <c r="K63" s="4"/>
-      <c r="L63" s="4"/>
-    </row>
-    <row r="64" spans="2:14">
-      <c r="B64" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C64" s="13"/>
-      <c r="D64" s="16">
-        <v>44.71</v>
-      </c>
-      <c r="E64" s="13"/>
-      <c r="F64" s="34"/>
-      <c r="G64" s="34"/>
-      <c r="H64" s="34">
-        <v>270.17</v>
-      </c>
-      <c r="I64" s="34"/>
-      <c r="J64" s="34"/>
-      <c r="K64" s="34"/>
-      <c r="L64" s="34"/>
-    </row>
-    <row r="65" spans="2:12">
-      <c r="B65" s="21" t="s">
+        <v>27.776110097674742</v>
+      </c>
+      <c r="I71" s="42"/>
+      <c r="J71" s="42"/>
+      <c r="K71" s="42"/>
+      <c r="L71" s="42"/>
+    </row>
+    <row r="72" spans="2:14" s="6" customFormat="1">
+      <c r="B72" s="22"/>
+      <c r="D72" s="28"/>
+      <c r="F72" s="28"/>
+      <c r="G72" s="28"/>
+      <c r="H72" s="28"/>
+      <c r="I72" s="28"/>
+      <c r="J72" s="28"/>
+      <c r="K72" s="28"/>
+      <c r="L72" s="28"/>
+      <c r="N72" s="19"/>
+    </row>
+    <row r="73" spans="2:14">
+      <c r="B73" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C73" s="13"/>
+      <c r="D73" s="16">
+        <v>39.409999999999997</v>
+      </c>
+      <c r="E73" s="13"/>
+      <c r="F73" s="31">
+        <v>58.13</v>
+      </c>
+      <c r="G73" s="31">
+        <v>88.5</v>
+      </c>
+      <c r="H73" s="31">
+        <v>190.09</v>
+      </c>
+      <c r="I73" s="31">
+        <v>346.53</v>
+      </c>
+      <c r="J73" s="31">
+        <v>606.28</v>
+      </c>
+      <c r="K73" s="31">
+        <v>1146.22</v>
+      </c>
+      <c r="L73" s="45" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="74" spans="2:14">
+      <c r="B74" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C65" s="13"/>
-      <c r="D65" s="32">
-        <f>D$6/D64</f>
-        <v>48132.364124356965</v>
-      </c>
-      <c r="E65" s="13"/>
-      <c r="F65" s="32" t="e">
-        <f t="shared" ref="F65:G65" si="22">F$6/F64</f>
+      <c r="C74" s="13"/>
+      <c r="D74" s="30">
+        <f>D$6/D73</f>
+        <v>54605.379345343827</v>
+      </c>
+      <c r="E74" s="13"/>
+      <c r="F74" s="30">
+        <f t="shared" ref="F74:K74" si="22">F$6/F73</f>
+        <v>3.1481162910717355</v>
+      </c>
+      <c r="G74" s="30">
+        <f t="shared" si="22"/>
+        <v>16.576271186440678</v>
+      </c>
+      <c r="H74" s="30">
+        <f t="shared" si="22"/>
+        <v>63.280551317796835</v>
+      </c>
+      <c r="I74" s="30">
+        <f t="shared" si="22"/>
+        <v>93.521484431362367</v>
+      </c>
+      <c r="J74" s="30">
+        <f t="shared" si="22"/>
+        <v>109.85353302104639</v>
+      </c>
+      <c r="K74" s="30">
+        <f t="shared" si="22"/>
+        <v>114.58533265865191</v>
+      </c>
+      <c r="L74" s="44"/>
+    </row>
+    <row r="75" spans="2:14" s="6" customFormat="1">
+      <c r="B75" s="22"/>
+      <c r="D75" s="28"/>
+      <c r="F75" s="28"/>
+      <c r="G75" s="28"/>
+      <c r="H75" s="28"/>
+      <c r="I75" s="28"/>
+      <c r="J75" s="28"/>
+      <c r="K75" s="28"/>
+      <c r="L75" s="44"/>
+      <c r="N75" s="19"/>
+    </row>
+    <row r="76" spans="2:14">
+      <c r="B76" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C76" s="13"/>
+      <c r="D76" s="16">
+        <v>39</v>
+      </c>
+      <c r="E76" s="13"/>
+      <c r="F76" s="31">
+        <v>77.11</v>
+      </c>
+      <c r="G76" s="31">
+        <v>162.76</v>
+      </c>
+      <c r="H76" s="31">
+        <v>270.76</v>
+      </c>
+      <c r="I76" s="31">
+        <v>395.53</v>
+      </c>
+      <c r="J76" s="31">
+        <v>601.86</v>
+      </c>
+      <c r="K76" s="31">
+        <v>1011.69</v>
+      </c>
+      <c r="L76" s="45" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="77" spans="2:14">
+      <c r="B77" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C77" s="13"/>
+      <c r="D77" s="30">
+        <f>D$6/D76</f>
+        <v>55179.435897435898</v>
+      </c>
+      <c r="E77" s="13"/>
+      <c r="F77" s="30">
+        <f t="shared" ref="F77:G77" si="23">F$6/F76</f>
+        <v>2.3732330437037996</v>
+      </c>
+      <c r="G77" s="30">
+        <f t="shared" si="23"/>
+        <v>9.0132710739739501</v>
+      </c>
+      <c r="H77" s="30">
+        <f t="shared" ref="H77:K77" si="24">H$6/H76</f>
+        <v>44.426798640862756</v>
+      </c>
+      <c r="I77" s="30">
+        <f t="shared" si="24"/>
+        <v>81.935630672768184</v>
+      </c>
+      <c r="J77" s="30">
+        <f t="shared" si="24"/>
+        <v>110.66028644535274</v>
+      </c>
+      <c r="K77" s="30">
+        <f t="shared" si="24"/>
+        <v>129.82237641965423</v>
+      </c>
+      <c r="L77" s="44"/>
+    </row>
+    <row r="78" spans="2:14" s="6" customFormat="1">
+      <c r="B78" s="22"/>
+      <c r="D78" s="28"/>
+      <c r="F78" s="28"/>
+      <c r="G78" s="28"/>
+      <c r="H78" s="28"/>
+      <c r="I78" s="28"/>
+      <c r="J78" s="28"/>
+      <c r="K78" s="28"/>
+      <c r="L78" s="28"/>
+      <c r="N78" s="19"/>
+    </row>
+    <row r="79" spans="2:14">
+      <c r="B79" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C79" s="13"/>
+      <c r="D79" s="16"/>
+      <c r="E79" s="13"/>
+      <c r="F79" s="46"/>
+      <c r="G79" s="46"/>
+      <c r="H79" s="46"/>
+      <c r="I79" s="46"/>
+      <c r="J79" s="46"/>
+      <c r="K79" s="46"/>
+      <c r="L79" s="31"/>
+    </row>
+    <row r="80" spans="2:14">
+      <c r="B80" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C80" s="13"/>
+      <c r="D80" s="30" t="e">
+        <f>D$6/D79</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G65" s="32" t="e">
-        <f t="shared" si="22"/>
+      <c r="E80" s="13"/>
+      <c r="F80" s="30" t="e">
+        <f t="shared" ref="F80:K80" si="25">F$6/F79</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H65" s="32">
-        <f>H$6/H64</f>
-        <v>44.523818336602879</v>
-      </c>
-      <c r="I65" s="32" t="e">
-        <f t="shared" ref="I65:K65" si="23">I$6/I64</f>
+      <c r="G80" s="30" t="e">
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J65" s="32" t="e">
-        <f t="shared" si="23"/>
+      <c r="H80" s="30" t="e">
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K65" s="32" t="e">
-        <f t="shared" si="23"/>
+      <c r="I80" s="30" t="e">
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L65" s="32"/>
-    </row>
-    <row r="66" spans="2:12">
-      <c r="B66" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C66" s="13"/>
-      <c r="D66" s="34">
-        <v>43.34</v>
-      </c>
-      <c r="E66" s="13"/>
-      <c r="F66" s="34">
-        <v>117.96</v>
-      </c>
-      <c r="G66" s="34">
-        <v>248.14</v>
-      </c>
-      <c r="H66" s="34">
-        <v>433.07</v>
-      </c>
-      <c r="I66" s="34"/>
-      <c r="J66" s="34"/>
-      <c r="K66" s="34"/>
-      <c r="L66" s="34"/>
-    </row>
-    <row r="67" spans="2:12">
-      <c r="B67" s="21" t="s">
+      <c r="J80" s="30" t="e">
+        <f t="shared" si="25"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K80" s="30" t="e">
+        <f t="shared" si="25"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L80" s="30"/>
+    </row>
+    <row r="81" spans="2:14" s="6" customFormat="1">
+      <c r="B81" s="22"/>
+      <c r="D81" s="28"/>
+      <c r="F81" s="28"/>
+      <c r="G81" s="28"/>
+      <c r="H81" s="28"/>
+      <c r="I81" s="28"/>
+      <c r="J81" s="28"/>
+      <c r="K81" s="28"/>
+      <c r="L81" s="28"/>
+      <c r="N81" s="19"/>
+    </row>
+    <row r="82" spans="2:14">
+      <c r="B82" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C82" s="13"/>
+      <c r="D82" s="16">
+        <v>34.67</v>
+      </c>
+      <c r="E82" s="13"/>
+      <c r="F82" s="31">
+        <v>70.25</v>
+      </c>
+      <c r="G82" s="31">
+        <v>142.19</v>
+      </c>
+      <c r="H82" s="31">
+        <v>223.97</v>
+      </c>
+      <c r="I82" s="31">
+        <v>272.47000000000003</v>
+      </c>
+      <c r="J82" s="31">
+        <v>322.70999999999998</v>
+      </c>
+      <c r="K82" s="31">
+        <v>454.26</v>
+      </c>
+      <c r="L82" s="31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="83" spans="2:14">
+      <c r="B83" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C67" s="13"/>
-      <c r="D67" s="32">
-        <f t="shared" ref="D67:I67" si="24">D$6/D66</f>
-        <v>49653.853253345638</v>
-      </c>
-      <c r="E67" s="13"/>
-      <c r="F67" s="32">
-        <f t="shared" si="24"/>
-        <v>1.5513733468972535</v>
-      </c>
-      <c r="G67" s="32">
-        <f t="shared" si="24"/>
-        <v>5.9119851696622874</v>
-      </c>
-      <c r="H67" s="32">
-        <f t="shared" si="24"/>
-        <v>27.776110097674742</v>
-      </c>
-      <c r="I67" s="32" t="e">
-        <f t="shared" si="24"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J67" s="32" t="e">
-        <f t="shared" ref="J67" si="25">J$6/J66</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K67" s="32" t="e">
-        <f t="shared" ref="K67" si="26">K$6/K66</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L67" s="32"/>
-    </row>
-    <row r="68" spans="2:12">
-      <c r="B68" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C68" s="13"/>
-      <c r="D68" s="16">
-        <v>39.409999999999997</v>
-      </c>
-      <c r="E68" s="13"/>
-      <c r="F68" s="34">
-        <v>58.13</v>
-      </c>
-      <c r="G68" s="34">
-        <v>88.5</v>
-      </c>
-      <c r="H68" s="34">
-        <v>190.09</v>
-      </c>
-      <c r="I68" s="34">
-        <v>346.53</v>
-      </c>
-      <c r="J68" s="34">
-        <v>606.28</v>
-      </c>
-      <c r="K68" s="34">
-        <v>1146.22</v>
-      </c>
-      <c r="L68" s="34"/>
-    </row>
-    <row r="69" spans="2:12">
-      <c r="B69" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C69" s="19"/>
-      <c r="D69" s="32">
-        <f>D$6/D68</f>
-        <v>54605.379345343827</v>
-      </c>
-      <c r="E69" s="13"/>
-      <c r="F69" s="32">
-        <f t="shared" ref="F69:K69" si="27">F$6/F68</f>
-        <v>3.1481162910717355</v>
-      </c>
-      <c r="G69" s="32">
-        <f t="shared" si="27"/>
-        <v>16.576271186440678</v>
-      </c>
-      <c r="H69" s="32">
-        <f t="shared" si="27"/>
-        <v>63.280551317796835</v>
-      </c>
-      <c r="I69" s="32">
-        <f t="shared" si="27"/>
-        <v>93.521484431362367</v>
-      </c>
-      <c r="J69" s="32">
-        <f t="shared" si="27"/>
-        <v>109.85353302104639</v>
-      </c>
-      <c r="K69" s="32">
-        <f t="shared" si="27"/>
-        <v>114.58533265865191</v>
-      </c>
-      <c r="L69" s="32"/>
-    </row>
-    <row r="70" spans="2:12">
-      <c r="B70" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C70" s="13"/>
-      <c r="D70" s="16">
-        <v>39</v>
-      </c>
-      <c r="E70" s="13"/>
-      <c r="F70" s="34">
-        <v>77.11</v>
-      </c>
-      <c r="G70" s="34">
-        <v>162.76</v>
-      </c>
-      <c r="H70" s="34">
-        <v>270.76</v>
-      </c>
-      <c r="I70" s="34">
-        <v>395.53</v>
-      </c>
-      <c r="J70" s="34">
-        <v>601.86</v>
-      </c>
-      <c r="K70" s="34">
-        <v>1011.69</v>
-      </c>
-      <c r="L70" s="34"/>
-    </row>
-    <row r="71" spans="2:12">
-      <c r="B71" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C71" s="13"/>
-      <c r="D71" s="32">
-        <f>D$6/D70</f>
-        <v>55179.435897435898</v>
-      </c>
-      <c r="E71" s="13"/>
-      <c r="F71" s="32">
-        <f t="shared" ref="F71:G71" si="28">F$6/F70</f>
-        <v>2.3732330437037996</v>
-      </c>
-      <c r="G71" s="32">
-        <f t="shared" si="28"/>
-        <v>9.0132710739739501</v>
-      </c>
-      <c r="H71" s="32">
-        <f t="shared" ref="H71:K71" si="29">H$6/H70</f>
-        <v>44.426798640862756</v>
-      </c>
-      <c r="I71" s="32">
-        <f t="shared" si="29"/>
-        <v>81.935630672768184</v>
-      </c>
-      <c r="J71" s="32">
-        <f t="shared" si="29"/>
-        <v>110.66028644535274</v>
-      </c>
-      <c r="K71" s="32">
-        <f t="shared" si="29"/>
-        <v>129.82237641965423</v>
-      </c>
-      <c r="L71" s="32"/>
-    </row>
-    <row r="72" spans="2:12">
-      <c r="B72" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="C72" s="13"/>
-      <c r="D72" s="16"/>
-      <c r="E72" s="13"/>
-      <c r="F72" s="34"/>
-      <c r="G72" s="34"/>
-      <c r="H72" s="34"/>
-      <c r="I72" s="34"/>
-      <c r="J72" s="34"/>
-      <c r="K72" s="34"/>
-      <c r="L72" s="34"/>
-    </row>
-    <row r="73" spans="2:12">
-      <c r="B73" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C73" s="19"/>
-      <c r="D73" s="32" t="e">
-        <f>D$6/D72</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E73" s="13"/>
-      <c r="F73" s="32" t="e">
-        <f t="shared" ref="F73:K73" si="30">F$6/F72</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G73" s="32" t="e">
-        <f t="shared" si="30"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H73" s="32" t="e">
-        <f t="shared" si="30"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I73" s="32" t="e">
-        <f t="shared" si="30"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J73" s="32" t="e">
-        <f t="shared" si="30"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K73" s="32" t="e">
-        <f t="shared" si="30"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L73" s="32"/>
-    </row>
-    <row r="74" spans="2:12">
-      <c r="B74" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C74" s="13"/>
-      <c r="D74" s="16"/>
-      <c r="E74" s="13"/>
-      <c r="F74" s="34"/>
-      <c r="G74" s="34"/>
-      <c r="H74" s="34"/>
-      <c r="I74" s="34"/>
-      <c r="J74" s="34"/>
-      <c r="K74" s="34"/>
-      <c r="L74" s="34"/>
-    </row>
-    <row r="75" spans="2:12">
-      <c r="B75" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C75" s="13"/>
-      <c r="D75" s="32" t="e">
-        <f>D$6/D74</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E75" s="13"/>
-      <c r="F75" s="32" t="e">
-        <f t="shared" ref="F75:K75" si="31">F$6/F74</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G75" s="32" t="e">
-        <f t="shared" si="31"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H75" s="32" t="e">
-        <f t="shared" si="31"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I75" s="32" t="e">
-        <f t="shared" si="31"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J75" s="32" t="e">
-        <f t="shared" si="31"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K75" s="32" t="e">
-        <f t="shared" si="31"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L75" s="32"/>
+      <c r="C83" s="13"/>
+      <c r="D83" s="30">
+        <f>D$6/D82</f>
+        <v>62070.897029131811</v>
+      </c>
+      <c r="E83" s="13"/>
+      <c r="F83" s="30">
+        <f t="shared" ref="F83:K83" si="26">F$6/F82</f>
+        <v>2.604982206405694</v>
+      </c>
+      <c r="G83" s="30">
+        <f t="shared" si="26"/>
+        <v>10.317181236373866</v>
+      </c>
+      <c r="H83" s="30">
+        <f t="shared" si="26"/>
+        <v>53.708085904362193</v>
+      </c>
+      <c r="I83" s="30">
+        <f t="shared" si="26"/>
+        <v>118.94153484787314</v>
+      </c>
+      <c r="J83" s="30">
+        <f t="shared" si="26"/>
+        <v>206.38344024046359</v>
+      </c>
+      <c r="K83" s="30">
+        <f t="shared" si="26"/>
+        <v>289.12957337207769</v>
+      </c>
+      <c r="L83" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>